<commit_message>
updated fis function.R and added fis pressures and resilience, registered layers, updated matrix for pressure and resilience
</commit_message>
<xml_diff>
--- a/prep/FIS/Fisheries_CSV_Layers/fish_scores_table.xlsx
+++ b/prep/FIS/Fisheries_CSV_Layers/fish_scores_table.xlsx
@@ -414,18 +414,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -437,9 +428,6 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -455,9 +443,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -471,6 +456,24 @@
     </xf>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,49 +778,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+    <sheetView tabSelected="1" topLeftCell="B39" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="3" width="21" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="18" style="5" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="19" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="21" style="18" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="5" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:9" s="10" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="21" t="s">
         <v>22</v>
       </c>
     </row>
@@ -825,28 +829,28 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="2">
         <v>2015</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="2">
         <v>1529</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="3">
         <v>0.60791740900000002</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2" s="15">
         <v>2.86538</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="4">
         <v>26.92333</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="4">
         <v>100</v>
       </c>
     </row>
@@ -854,24 +858,24 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="5">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="2">
         <v>2014</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="2">
         <v>1738</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="3">
         <v>0.60791740900000002</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="15">
         <v>2.8543799999999999</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="4">
         <v>27.53444</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="4">
         <v>100</v>
       </c>
     </row>
@@ -879,24 +883,24 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="5">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="2">
         <v>2013</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="2">
         <v>1565</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="3">
         <v>0.60791740900000002</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="15">
         <v>2.86</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="4">
         <v>27.222220000000004</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="4">
         <v>100</v>
       </c>
     </row>
@@ -904,24 +908,24 @@
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="5">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="2">
         <v>2012</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="2">
         <v>1684</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="3">
         <v>0.60791740900000002</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="15">
         <v>2.56</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="4">
         <v>43.888890000000004</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="4">
         <v>100</v>
       </c>
     </row>
@@ -929,24 +933,24 @@
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="5">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="2">
         <v>2011</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="2">
         <v>1669</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="3">
         <v>0.60791740900000002</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="15">
         <v>2.97</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="4">
         <v>21.11111</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="4">
         <v>100</v>
       </c>
     </row>
@@ -954,28 +958,28 @@
       <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="2">
         <v>2015</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="2">
         <v>807</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="3">
         <v>0.23447712400000001</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="15">
         <v>1.237773</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="4">
         <v>100</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="4">
         <v>100</v>
       </c>
     </row>
@@ -983,24 +987,24 @@
       <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="5">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="2">
         <v>2014</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="2">
         <v>705</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="3">
         <v>0.23447712400000001</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="15">
         <v>1.2602580000000001</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="4">
         <v>100</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1008,24 +1012,24 @@
       <c r="A9" s="1">
         <v>1</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="5">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="2">
         <v>2013</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="2">
         <v>500</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="3">
         <v>0.23447712400000001</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="15">
         <v>1.282743</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="4">
         <v>100</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1033,24 +1037,24 @@
       <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="5">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="2">
         <v>2012</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="2">
         <v>549</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="3">
         <v>0.23447712400000001</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="15">
         <v>1.22</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="4">
         <v>100</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1058,24 +1062,24 @@
       <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="5">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="2">
         <v>2011</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="2">
         <v>596</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="3">
         <v>0.23447712400000001</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="15">
         <v>1.3</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="4">
         <v>100</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1083,28 +1087,28 @@
       <c r="A12" s="1">
         <v>1</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="2">
         <v>2015</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="2">
         <v>59</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="3">
         <v>2.0202020000000001E-2</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="15">
         <v>0.82359700000000002</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="4">
         <v>100</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1112,24 +1116,24 @@
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="5">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="2">
         <v>2014</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="2">
         <v>58</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="3">
         <v>2.0202020000000001E-2</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="15">
         <v>0.84751799999999999</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="4">
         <v>100</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1137,24 +1141,24 @@
       <c r="A14" s="1">
         <v>1</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="5">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="2">
         <v>2013</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="2">
         <v>57</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="3">
         <v>2.0202020000000001E-2</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="15">
         <v>0.87143899999999996</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="4">
         <v>100</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1162,24 +1166,24 @@
       <c r="A15" s="1">
         <v>1</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="5">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="2">
         <v>2012</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="2">
         <v>50</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="3">
         <v>2.0202020000000001E-2</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="15">
         <v>0.79</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="4">
         <v>98.75</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="4">
         <v>98.75</v>
       </c>
     </row>
@@ -1187,24 +1191,24 @@
       <c r="A16" s="1">
         <v>1</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="5">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="2">
         <v>2011</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="2">
         <v>48</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="3">
         <v>2.0202020000000001E-2</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="15">
         <v>0.86</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="4">
         <v>100</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1212,28 +1216,28 @@
       <c r="A17" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="2">
         <v>2015</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="2">
         <v>9</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="3">
         <v>3.8621509999999999E-3</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="15">
         <v>0.98799999999999999</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="4">
         <v>100</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1241,24 +1245,24 @@
       <c r="A18" s="1">
         <v>1</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="5">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="2">
         <v>2014</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="2">
         <v>12</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="3">
         <v>3.8621509999999999E-3</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="15">
         <v>1.1415299999999999</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="4">
         <v>100</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1266,24 +1270,24 @@
       <c r="A19" s="1">
         <v>1</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="5">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="2">
         <v>2013</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="2">
         <v>8</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="3">
         <v>3.8621509999999999E-3</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="15">
         <v>1.2950600000000001</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="4">
         <v>100</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1291,24 +1295,24 @@
       <c r="A20" s="1">
         <v>1</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="5">
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="2">
         <v>2012</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="2">
         <v>11</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="3">
         <v>3.8621509999999999E-3</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="15">
         <v>1.2</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="4">
         <v>100</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1316,24 +1320,24 @@
       <c r="A21" s="1">
         <v>1</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="5">
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="2">
         <v>2011</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="2">
         <v>12</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="3">
         <v>3.8621509999999999E-3</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="15">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="4">
         <v>100</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="4">
         <v>100</v>
       </c>
     </row>
@@ -1341,28 +1345,28 @@
       <c r="A22" s="1">
         <v>1</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="2">
         <v>2015</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="2">
         <v>53</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="3">
         <v>2.0499109000000001E-2</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="15">
         <v>0.36166670000000001</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="4">
         <v>45.208330000000004</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="4">
         <v>45.208330000000004</v>
       </c>
     </row>
@@ -1370,24 +1374,24 @@
       <c r="A23" s="1">
         <v>1</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="5">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="2">
         <v>2014</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="2">
         <v>48</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="3">
         <v>2.0499109000000001E-2</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="15">
         <v>0.35599999999999998</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="4">
         <v>44.5</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="4">
         <v>44.5</v>
       </c>
     </row>
@@ -1395,24 +1399,24 @@
       <c r="A24" s="1">
         <v>1</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="5">
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="2">
         <v>2013</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="2">
         <v>44</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="3">
         <v>2.0499109000000001E-2</v>
       </c>
-      <c r="G24" s="20">
+      <c r="G24" s="15">
         <v>0.39</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="4">
         <v>48.75</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="4">
         <v>48.75</v>
       </c>
     </row>
@@ -1420,24 +1424,24 @@
       <c r="A25" s="1">
         <v>1</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="5">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="2">
         <v>2012</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="2">
         <v>58</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="3">
         <v>2.0499109000000001E-2</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="15">
         <v>0.36</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="4">
         <v>45</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="4">
         <v>45</v>
       </c>
     </row>
@@ -1445,24 +1449,24 @@
       <c r="A26" s="1">
         <v>1</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="5">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="2">
         <v>2011</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="2">
         <v>73</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="3">
         <v>2.0499109000000001E-2</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="15">
         <v>0.31</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="4">
         <v>38.75</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="4">
         <v>38.75</v>
       </c>
     </row>
@@ -1470,28 +1474,28 @@
       <c r="A27" s="1">
         <v>1</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="2">
         <v>2015</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="2">
         <v>21</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="3">
         <v>9.0612000000000002E-3</v>
       </c>
-      <c r="G27" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H27" s="7">
-        <v>75</v>
-      </c>
-      <c r="I27" s="7">
+      <c r="G27" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="4">
+        <v>75</v>
+      </c>
+      <c r="I27" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1499,24 +1503,24 @@
       <c r="A28" s="1">
         <v>1</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="5">
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="2">
         <v>2014</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="2">
         <v>41</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="3">
         <v>9.0612000000000002E-3</v>
       </c>
-      <c r="G28" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H28" s="7">
-        <v>75</v>
-      </c>
-      <c r="I28" s="7">
+      <c r="G28" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="4">
+        <v>75</v>
+      </c>
+      <c r="I28" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1524,24 +1528,24 @@
       <c r="A29" s="1">
         <v>1</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="5">
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="2">
         <v>2013</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="2">
         <v>17</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="3">
         <v>9.0612000000000002E-3</v>
       </c>
-      <c r="G29" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H29" s="7">
-        <v>75</v>
-      </c>
-      <c r="I29" s="7">
+      <c r="G29" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="4">
+        <v>75</v>
+      </c>
+      <c r="I29" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1549,24 +1553,24 @@
       <c r="A30" s="1">
         <v>1</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="5">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="2">
         <v>2012</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="2">
         <v>16</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="3">
         <v>9.0612000000000002E-3</v>
       </c>
-      <c r="G30" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H30" s="7">
+      <c r="G30" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="4">
         <v>74.0625</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1574,24 +1578,24 @@
       <c r="A31" s="1">
         <v>1</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="5">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="2">
         <v>2011</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="2">
         <v>27</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="3">
         <v>9.0612000000000002E-3</v>
       </c>
-      <c r="G31" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H31" s="7">
-        <v>75</v>
-      </c>
-      <c r="I31" s="7">
+      <c r="G31" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H31" s="4">
+        <v>75</v>
+      </c>
+      <c r="I31" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1599,28 +1603,28 @@
       <c r="A32" s="1">
         <v>1</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="2">
         <v>2015</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="2">
         <v>32</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="3">
         <v>1.4334522000000001E-2</v>
       </c>
-      <c r="G32" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H32" s="7">
-        <v>75</v>
-      </c>
-      <c r="I32" s="7">
+      <c r="G32" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="4">
+        <v>75</v>
+      </c>
+      <c r="I32" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1628,24 +1632,24 @@
       <c r="A33" s="1">
         <v>1</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="5">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="2">
         <v>2014</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="2">
         <v>35</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="3">
         <v>1.4334522000000001E-2</v>
       </c>
-      <c r="G33" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H33" s="7">
-        <v>75</v>
-      </c>
-      <c r="I33" s="7">
+      <c r="G33" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="4">
+        <v>75</v>
+      </c>
+      <c r="I33" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1653,24 +1657,24 @@
       <c r="A34" s="1">
         <v>1</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="5">
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="2">
         <v>2013</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="2">
         <v>35</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="3">
         <v>1.4334522000000001E-2</v>
       </c>
-      <c r="G34" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H34" s="7">
-        <v>75</v>
-      </c>
-      <c r="I34" s="7">
+      <c r="G34" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="4">
+        <v>75</v>
+      </c>
+      <c r="I34" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1678,24 +1682,24 @@
       <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="5">
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="2">
         <v>2012</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="2">
         <v>43</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="3">
         <v>1.4334522000000001E-2</v>
       </c>
-      <c r="G35" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H35" s="7">
+      <c r="G35" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" s="4">
         <v>74.0625</v>
       </c>
-      <c r="I35" s="7">
+      <c r="I35" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1703,24 +1707,24 @@
       <c r="A36" s="1">
         <v>1</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="5">
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="2">
         <v>2011</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="2">
         <v>48</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="3">
         <v>1.4334522000000001E-2</v>
       </c>
-      <c r="G36" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H36" s="7">
-        <v>75</v>
-      </c>
-      <c r="I36" s="7">
+      <c r="G36" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" s="4">
+        <v>75</v>
+      </c>
+      <c r="I36" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1728,28 +1732,28 @@
       <c r="A37" s="1">
         <v>1</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="2">
         <v>2015</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="2">
         <v>24</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="3">
         <v>1.3888889E-2</v>
       </c>
-      <c r="G37" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H37" s="7">
-        <v>75</v>
-      </c>
-      <c r="I37" s="7">
+      <c r="G37" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H37" s="4">
+        <v>75</v>
+      </c>
+      <c r="I37" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1757,24 +1761,24 @@
       <c r="A38" s="1">
         <v>1</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="5">
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="2">
         <v>2014</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="2">
         <v>41</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="3">
         <v>1.3888889E-2</v>
       </c>
-      <c r="G38" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H38" s="7">
-        <v>75</v>
-      </c>
-      <c r="I38" s="7">
+      <c r="G38" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H38" s="4">
+        <v>75</v>
+      </c>
+      <c r="I38" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1782,24 +1786,24 @@
       <c r="A39" s="1">
         <v>1</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="5">
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="2">
         <v>2013</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="2">
         <v>36</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="3">
         <v>1.3888889E-2</v>
       </c>
-      <c r="G39" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H39" s="7">
-        <v>75</v>
-      </c>
-      <c r="I39" s="7">
+      <c r="G39" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H39" s="4">
+        <v>75</v>
+      </c>
+      <c r="I39" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1807,24 +1811,24 @@
       <c r="A40" s="1">
         <v>1</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="5">
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="2">
         <v>2012</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="2">
         <v>35</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="3">
         <v>1.3888889E-2</v>
       </c>
-      <c r="G40" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H40" s="7">
+      <c r="G40" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H40" s="4">
         <v>74.0625</v>
       </c>
-      <c r="I40" s="7">
+      <c r="I40" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1832,24 +1836,24 @@
       <c r="A41" s="1">
         <v>1</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="5">
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="2">
         <v>2011</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="2">
         <v>51</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="3">
         <v>1.3888889E-2</v>
       </c>
-      <c r="G41" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H41" s="7">
-        <v>75</v>
-      </c>
-      <c r="I41" s="7">
+      <c r="G41" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H41" s="4">
+        <v>75</v>
+      </c>
+      <c r="I41" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1857,28 +1861,28 @@
       <c r="A42" s="1">
         <v>1</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="2">
         <v>2015</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="2">
         <v>53</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42" s="3">
         <v>2.8149138000000001E-2</v>
       </c>
-      <c r="G42" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H42" s="7">
-        <v>75</v>
-      </c>
-      <c r="I42" s="7">
+      <c r="G42" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H42" s="4">
+        <v>75</v>
+      </c>
+      <c r="I42" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1886,24 +1890,24 @@
       <c r="A43" s="1">
         <v>1</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="5">
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="2">
         <v>2014</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="2">
         <v>99</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="3">
         <v>2.8149138000000001E-2</v>
       </c>
-      <c r="G43" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H43" s="7">
-        <v>75</v>
-      </c>
-      <c r="I43" s="7">
+      <c r="G43" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H43" s="4">
+        <v>75</v>
+      </c>
+      <c r="I43" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1911,24 +1915,24 @@
       <c r="A44" s="1">
         <v>1</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="5">
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="2">
         <v>2013</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="2">
         <v>79</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="3">
         <v>2.8149138000000001E-2</v>
       </c>
-      <c r="G44" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H44" s="7">
-        <v>75</v>
-      </c>
-      <c r="I44" s="7">
+      <c r="G44" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H44" s="4">
+        <v>75</v>
+      </c>
+      <c r="I44" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1936,24 +1940,24 @@
       <c r="A45" s="1">
         <v>1</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="5">
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="2">
         <v>2012</v>
       </c>
-      <c r="E45" s="5">
-        <v>75</v>
-      </c>
-      <c r="F45" s="6">
+      <c r="E45" s="2">
+        <v>75</v>
+      </c>
+      <c r="F45" s="3">
         <v>2.8149138000000001E-2</v>
       </c>
-      <c r="G45" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H45" s="7">
+      <c r="G45" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H45" s="4">
         <v>74.0625</v>
       </c>
-      <c r="I45" s="7">
+      <c r="I45" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1961,24 +1965,24 @@
       <c r="A46" s="1">
         <v>1</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="5">
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="2">
         <v>2011</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="2">
         <v>73</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="3">
         <v>2.8149138000000001E-2</v>
       </c>
-      <c r="G46" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H46" s="7">
-        <v>75</v>
-      </c>
-      <c r="I46" s="7">
+      <c r="G46" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H46" s="4">
+        <v>75</v>
+      </c>
+      <c r="I46" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1986,28 +1990,28 @@
       <c r="A47" s="1">
         <v>1</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="2">
         <v>2015</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="2">
         <v>98</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="3">
         <v>4.0923945000000003E-2</v>
       </c>
-      <c r="G47" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H47" s="7">
-        <v>75</v>
-      </c>
-      <c r="I47" s="7">
+      <c r="G47" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H47" s="4">
+        <v>75</v>
+      </c>
+      <c r="I47" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2015,24 +2019,24 @@
       <c r="A48" s="1">
         <v>1</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="5">
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="2">
         <v>2014</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="2">
         <v>150</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="3">
         <v>4.0923945000000003E-2</v>
       </c>
-      <c r="G48" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H48" s="7">
-        <v>75</v>
-      </c>
-      <c r="I48" s="7">
+      <c r="G48" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H48" s="4">
+        <v>75</v>
+      </c>
+      <c r="I48" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2040,24 +2044,24 @@
       <c r="A49" s="1">
         <v>1</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="5">
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="2">
         <v>2013</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="2">
         <v>91</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F49" s="3">
         <v>4.0923945000000003E-2</v>
       </c>
-      <c r="G49" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H49" s="7">
-        <v>75</v>
-      </c>
-      <c r="I49" s="7">
+      <c r="G49" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H49" s="4">
+        <v>75</v>
+      </c>
+      <c r="I49" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2065,24 +2069,24 @@
       <c r="A50" s="1">
         <v>1</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="5">
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="2">
         <v>2012</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="2">
         <v>95</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F50" s="3">
         <v>4.0923945000000003E-2</v>
       </c>
-      <c r="G50" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H50" s="7">
+      <c r="G50" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H50" s="4">
         <v>74.0625</v>
       </c>
-      <c r="I50" s="7">
+      <c r="I50" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2090,24 +2094,24 @@
       <c r="A51" s="1">
         <v>1</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="5">
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="2">
         <v>2011</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="2">
         <v>117</v>
       </c>
-      <c r="F51" s="6">
+      <c r="F51" s="3">
         <v>4.0923945000000003E-2</v>
       </c>
-      <c r="G51" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H51" s="7">
-        <v>75</v>
-      </c>
-      <c r="I51" s="7">
+      <c r="G51" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H51" s="4">
+        <v>75</v>
+      </c>
+      <c r="I51" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2115,28 +2119,28 @@
       <c r="A52" s="1">
         <v>1</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D52" s="2">
         <v>2015</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="2">
         <v>6</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F52" s="3">
         <v>2.1538920000000001E-3</v>
       </c>
-      <c r="G52" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H52" s="7">
-        <v>75</v>
-      </c>
-      <c r="I52" s="7">
+      <c r="G52" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H52" s="4">
+        <v>75</v>
+      </c>
+      <c r="I52" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2144,24 +2148,24 @@
       <c r="A53" s="1">
         <v>1</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="5">
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="2">
         <v>2014</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E53" s="2">
         <v>6</v>
       </c>
-      <c r="F53" s="6">
+      <c r="F53" s="3">
         <v>2.1538920000000001E-3</v>
       </c>
-      <c r="G53" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H53" s="7">
-        <v>75</v>
-      </c>
-      <c r="I53" s="7">
+      <c r="G53" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H53" s="4">
+        <v>75</v>
+      </c>
+      <c r="I53" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2169,24 +2173,24 @@
       <c r="A54" s="1">
         <v>1</v>
       </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="5">
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="2">
         <v>2013</v>
       </c>
-      <c r="E54" s="5">
+      <c r="E54" s="2">
         <v>5</v>
       </c>
-      <c r="F54" s="6">
+      <c r="F54" s="3">
         <v>2.1538920000000001E-3</v>
       </c>
-      <c r="G54" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H54" s="7">
-        <v>75</v>
-      </c>
-      <c r="I54" s="7">
+      <c r="G54" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H54" s="4">
+        <v>75</v>
+      </c>
+      <c r="I54" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2194,24 +2198,24 @@
       <c r="A55" s="1">
         <v>1</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="5">
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="2">
         <v>2012</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55" s="2">
         <v>5</v>
       </c>
-      <c r="F55" s="6">
+      <c r="F55" s="3">
         <v>2.1538920000000001E-3</v>
       </c>
-      <c r="G55" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H55" s="7">
+      <c r="G55" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H55" s="4">
         <v>74.0625</v>
       </c>
-      <c r="I55" s="7">
+      <c r="I55" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2219,24 +2223,24 @@
       <c r="A56" s="1">
         <v>1</v>
       </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="5">
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="2">
         <v>2011</v>
       </c>
-      <c r="E56" s="5">
+      <c r="E56" s="2">
         <v>7</v>
       </c>
-      <c r="F56" s="6">
+      <c r="F56" s="3">
         <v>2.1538920000000001E-3</v>
       </c>
-      <c r="G56" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H56" s="7">
-        <v>75</v>
-      </c>
-      <c r="I56" s="7">
+      <c r="G56" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H56" s="4">
+        <v>75</v>
+      </c>
+      <c r="I56" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2244,28 +2248,28 @@
       <c r="A57" s="1">
         <v>1</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D57" s="5">
+      <c r="D57" s="2">
         <v>2015</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E57" s="2">
         <v>11</v>
       </c>
-      <c r="F57" s="6">
+      <c r="F57" s="3">
         <v>4.5306000000000001E-3</v>
       </c>
-      <c r="G57" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H57" s="7">
-        <v>75</v>
-      </c>
-      <c r="I57" s="7">
+      <c r="G57" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H57" s="4">
+        <v>75</v>
+      </c>
+      <c r="I57" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2273,24 +2277,24 @@
       <c r="A58" s="1">
         <v>1</v>
       </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="5">
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="2">
         <v>2014</v>
       </c>
-      <c r="E58" s="5">
+      <c r="E58" s="2">
         <v>15</v>
       </c>
-      <c r="F58" s="6">
+      <c r="F58" s="3">
         <v>4.5306000000000001E-3</v>
       </c>
-      <c r="G58" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H58" s="7">
-        <v>75</v>
-      </c>
-      <c r="I58" s="7">
+      <c r="G58" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H58" s="4">
+        <v>75</v>
+      </c>
+      <c r="I58" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2298,24 +2302,24 @@
       <c r="A59" s="1">
         <v>1</v>
       </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="5">
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="2">
         <v>2013</v>
       </c>
-      <c r="E59" s="5">
+      <c r="E59" s="2">
         <v>13</v>
       </c>
-      <c r="F59" s="6">
+      <c r="F59" s="3">
         <v>4.5306000000000001E-3</v>
       </c>
-      <c r="G59" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H59" s="7">
-        <v>75</v>
-      </c>
-      <c r="I59" s="7">
+      <c r="G59" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H59" s="4">
+        <v>75</v>
+      </c>
+      <c r="I59" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2323,24 +2327,24 @@
       <c r="A60" s="1">
         <v>1</v>
       </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="5">
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="2">
         <v>2012</v>
       </c>
-      <c r="E60" s="5">
+      <c r="E60" s="2">
         <v>9</v>
       </c>
-      <c r="F60" s="6">
+      <c r="F60" s="3">
         <v>4.5306000000000001E-3</v>
       </c>
-      <c r="G60" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H60" s="7">
+      <c r="G60" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H60" s="4">
         <v>74.0625</v>
       </c>
-      <c r="I60" s="7">
+      <c r="I60" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2348,24 +2352,24 @@
       <c r="A61" s="1">
         <v>1</v>
       </c>
-      <c r="B61" s="15"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="16">
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="11">
         <v>2011</v>
       </c>
-      <c r="E61" s="16">
+      <c r="E61" s="11">
         <v>13</v>
       </c>
-      <c r="F61" s="17">
+      <c r="F61" s="12">
         <v>4.5306000000000001E-3</v>
       </c>
-      <c r="G61" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="H61" s="18">
-        <v>75</v>
-      </c>
-      <c r="I61" s="18">
+      <c r="G61" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H61" s="13">
+        <v>75</v>
+      </c>
+      <c r="I61" s="13">
         <v>75</v>
       </c>
     </row>
@@ -2412,7 +2416,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="6" t="s">
         <v>98</v>
       </c>
       <c r="B1" t="s">
@@ -2432,7 +2436,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B2">
@@ -2452,7 +2456,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B3">
@@ -2472,7 +2476,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B4">
@@ -2492,7 +2496,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B5">
@@ -2512,7 +2516,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B6">
@@ -2532,7 +2536,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B7">
@@ -2552,7 +2556,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B8">
@@ -2572,7 +2576,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B9">
@@ -2592,7 +2596,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B10">
@@ -2612,7 +2616,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B11">
@@ -2632,7 +2636,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B12">
@@ -2652,7 +2656,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B13">
@@ -2672,7 +2676,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B14">
@@ -2692,7 +2696,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B15">
@@ -2712,7 +2716,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B16">
@@ -2732,7 +2736,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B17">
@@ -2752,7 +2756,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
       <c r="B18">
@@ -2772,7 +2776,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B19">
@@ -2792,7 +2796,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B20">
@@ -2812,7 +2816,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B21">
@@ -2832,7 +2836,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B22">
@@ -2852,7 +2856,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B23">
@@ -2872,7 +2876,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B24">
@@ -2892,7 +2896,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B25">
@@ -2912,7 +2916,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B26">
@@ -2932,7 +2936,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B27">
@@ -2952,7 +2956,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B28">
@@ -2972,7 +2976,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B29">
@@ -2992,7 +2996,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B30">
@@ -3012,7 +3016,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B31">
@@ -3032,7 +3036,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B32">
@@ -3052,7 +3056,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="7" t="s">
         <v>68</v>
       </c>
       <c r="B33">
@@ -3072,7 +3076,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B34">
@@ -3092,7 +3096,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B35">
@@ -3112,7 +3116,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B36">
@@ -3132,7 +3136,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B37">
@@ -3152,7 +3156,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B38">
@@ -3172,7 +3176,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B39">
@@ -3192,7 +3196,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B40">
@@ -3212,7 +3216,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B41">
@@ -3232,7 +3236,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B42">
@@ -3252,7 +3256,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B43">
@@ -3272,7 +3276,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B44">
@@ -3292,7 +3296,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="7" t="s">
         <v>80</v>
       </c>
       <c r="B45">
@@ -3312,7 +3316,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B46">
@@ -3332,7 +3336,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B47">
@@ -3352,7 +3356,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B48">
@@ -3372,7 +3376,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B49">
@@ -3392,7 +3396,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B50">
@@ -3412,7 +3416,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B51">
@@ -3432,7 +3436,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="7" t="s">
         <v>87</v>
       </c>
       <c r="B52">
@@ -3452,7 +3456,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B53">
@@ -3472,7 +3476,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B54">
@@ -3492,7 +3496,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="7" t="s">
         <v>90</v>
       </c>
       <c r="B55">
@@ -3512,7 +3516,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B56">
@@ -3532,7 +3536,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B57">
@@ -3552,7 +3556,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B58">
@@ -3572,7 +3576,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="7" t="s">
         <v>94</v>
       </c>
       <c r="B59">
@@ -3592,7 +3596,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="7" t="s">
         <v>95</v>
       </c>
       <c r="B60">
@@ -3612,7 +3616,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B61">
@@ -3632,15 +3636,15 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="7" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
+      <c r="A63" s="8"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="9" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3660,7 +3664,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
+      <c r="A1" s="7"/>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3687,7 +3691,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2">
@@ -3716,7 +3720,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3">
@@ -3745,7 +3749,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4">
@@ -3774,7 +3778,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5">
@@ -3803,7 +3807,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6">
@@ -3832,7 +3836,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7">
@@ -3861,7 +3865,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8">
@@ -3890,7 +3894,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9">
@@ -3919,7 +3923,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10">
@@ -3948,7 +3952,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11">
@@ -3977,7 +3981,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12">
@@ -4006,7 +4010,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13">
@@ -4035,7 +4039,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14">
@@ -4064,7 +4068,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15">
@@ -4093,7 +4097,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16">
@@ -4122,7 +4126,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17">
@@ -4151,7 +4155,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18">
@@ -4180,7 +4184,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19">
@@ -4209,7 +4213,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20">
@@ -4238,7 +4242,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21">
@@ -4267,7 +4271,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+      <c r="A22" s="7">
         <v>21</v>
       </c>
       <c r="B22">
@@ -4296,7 +4300,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="A23" s="7">
         <v>22</v>
       </c>
       <c r="B23">
@@ -4325,7 +4329,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+      <c r="A24" s="7">
         <v>23</v>
       </c>
       <c r="B24">
@@ -4354,7 +4358,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25">
@@ -4383,7 +4387,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="A26" s="7">
         <v>25</v>
       </c>
       <c r="B26">
@@ -4412,7 +4416,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
+      <c r="A27" s="7">
         <v>26</v>
       </c>
       <c r="B27">
@@ -4441,7 +4445,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="A28" s="7">
         <v>27</v>
       </c>
       <c r="B28">
@@ -4470,7 +4474,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
+      <c r="A29" s="7">
         <v>28</v>
       </c>
       <c r="B29">
@@ -4499,7 +4503,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+      <c r="A30" s="7">
         <v>29</v>
       </c>
       <c r="B30">
@@ -4528,7 +4532,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
+      <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31">
@@ -4557,7 +4561,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
+      <c r="A32" s="7">
         <v>31</v>
       </c>
       <c r="B32">
@@ -4586,7 +4590,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="11">
+      <c r="A33" s="7">
         <v>32</v>
       </c>
       <c r="B33">
@@ -4615,7 +4619,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
+      <c r="A34" s="7">
         <v>33</v>
       </c>
       <c r="B34">
@@ -4644,7 +4648,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
+      <c r="A35" s="7">
         <v>34</v>
       </c>
       <c r="B35">
@@ -4673,7 +4677,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="11">
+      <c r="A36" s="7">
         <v>35</v>
       </c>
       <c r="B36">
@@ -4702,7 +4706,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+      <c r="A37" s="7">
         <v>36</v>
       </c>
       <c r="B37">
@@ -4731,7 +4735,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="A38" s="7">
         <v>37</v>
       </c>
       <c r="B38">
@@ -4760,7 +4764,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="11">
+      <c r="A39" s="7">
         <v>38</v>
       </c>
       <c r="B39">
@@ -4789,7 +4793,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
+      <c r="A40" s="7">
         <v>39</v>
       </c>
       <c r="B40">
@@ -4818,7 +4822,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="11">
+      <c r="A41" s="7">
         <v>40</v>
       </c>
       <c r="B41">
@@ -4847,7 +4851,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="11">
+      <c r="A42" s="7">
         <v>41</v>
       </c>
       <c r="B42">
@@ -4876,7 +4880,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="11">
+      <c r="A43" s="7">
         <v>42</v>
       </c>
       <c r="B43">
@@ -4905,7 +4909,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="11">
+      <c r="A44" s="7">
         <v>43</v>
       </c>
       <c r="B44">
@@ -4934,7 +4938,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
+      <c r="A45" s="7">
         <v>44</v>
       </c>
       <c r="B45">
@@ -4963,7 +4967,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="11">
+      <c r="A46" s="7">
         <v>45</v>
       </c>
       <c r="B46">
@@ -4992,7 +4996,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
+      <c r="A47" s="7">
         <v>46</v>
       </c>
       <c r="B47">
@@ -5021,7 +5025,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="11">
+      <c r="A48" s="7">
         <v>47</v>
       </c>
       <c r="B48">
@@ -5050,7 +5054,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
+      <c r="A49" s="7">
         <v>48</v>
       </c>
       <c r="B49">
@@ -5079,7 +5083,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
+      <c r="A50" s="7">
         <v>49</v>
       </c>
       <c r="B50">
@@ -5108,7 +5112,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="11">
+      <c r="A51" s="7">
         <v>50</v>
       </c>
       <c r="B51">
@@ -5137,7 +5141,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="11">
+      <c r="A52" s="7">
         <v>51</v>
       </c>
       <c r="B52">
@@ -5166,7 +5170,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="11">
+      <c r="A53" s="7">
         <v>52</v>
       </c>
       <c r="B53">
@@ -5195,7 +5199,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="11">
+      <c r="A54" s="7">
         <v>53</v>
       </c>
       <c r="B54">
@@ -5224,7 +5228,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="11">
+      <c r="A55" s="7">
         <v>54</v>
       </c>
       <c r="B55">
@@ -5253,7 +5257,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="11">
+      <c r="A56" s="7">
         <v>55</v>
       </c>
       <c r="B56">
@@ -5282,7 +5286,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="11">
+      <c r="A57" s="7">
         <v>56</v>
       </c>
       <c r="B57">
@@ -5311,7 +5315,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="11">
+      <c r="A58" s="7">
         <v>57</v>
       </c>
       <c r="B58">
@@ -5340,7 +5344,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="11">
+      <c r="A59" s="7">
         <v>58</v>
       </c>
       <c r="B59">
@@ -5369,7 +5373,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="11">
+      <c r="A60" s="7">
         <v>59</v>
       </c>
       <c r="B60">
@@ -5398,7 +5402,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="11">
+      <c r="A61" s="7">
         <v>60</v>
       </c>
       <c r="B61">
@@ -5427,10 +5431,10 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="12"/>
+      <c r="A62" s="8"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="9" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>